<commit_message>
fixed ion channel naming
</commit_message>
<xml_diff>
--- a/data/Gene_list.xlsx
+++ b/data/Gene_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbunga/gitHub/panacea-rnaseq/woolf_sensory_ampliseq/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927FE62A-FCE0-1C48-854E-638400F3C732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D4E576-E5F5-034E-8E00-2AE4B594FE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10340" yWindow="540" windowWidth="35840" windowHeight="21940" activeTab="2" xr2:uid="{6D36EDA0-D1D8-4E41-872E-A4F8180D8D28}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="2" xr2:uid="{6D36EDA0-D1D8-4E41-872E-A4F8180D8D28}"/>
   </bookViews>
   <sheets>
     <sheet name="Previous list" sheetId="1" r:id="rId1"/>
@@ -1237,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{651FB150-DEEC-6B42-A5E6-2F439B22C97C}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="200" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1488,7 +1488,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
         <v>46</v>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
         <v>47</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
         <v>48</v>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
         <v>49</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
         <v>50</v>
@@ -1528,7 +1528,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
         <v>51</v>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B37" t="s">
         <v>52</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
         <v>53</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
         <v>54</v>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
         <v>24</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
         <v>61</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
         <v>56</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B44" t="s">
         <v>62</v>

</xml_diff>